<commit_message>
Fixes competencias, entrenamientos, ortograficos
</commit_message>
<xml_diff>
--- a/cp.xlsx
+++ b/cp.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="243">
   <si>
     <t>rsca4321@gmail.com</t>
   </si>
@@ -740,6 +740,24 @@
   </si>
   <si>
     <t>C5</t>
+  </si>
+  <si>
+    <t>Futbol Delantero</t>
+  </si>
+  <si>
+    <t>Tiros a Gol,  Tiros. Pases, Faltas, Goles</t>
+  </si>
+  <si>
+    <t>Futbol Medio Campo</t>
+  </si>
+  <si>
+    <t>Pases, Centros, Goles, Faltas, Kilometros corridos</t>
+  </si>
+  <si>
+    <t>Faltas, Pases, Barridas, Recuperaciones</t>
+  </si>
+  <si>
+    <t>Paradas, Saques de meta, Faltas</t>
   </si>
 </sst>
 </file>
@@ -882,19 +900,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -906,14 +912,8 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -921,22 +921,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -946,6 +934,36 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2352,7 +2370,7 @@
   <dimension ref="B3:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2565,6 +2583,9 @@
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>237</v>
+      </c>
       <c r="N15">
         <v>27485124</v>
       </c>
@@ -2585,6 +2606,9 @@
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>238</v>
+      </c>
       <c r="N16">
         <v>29854754</v>
       </c>
@@ -2601,7 +2625,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>239</v>
+      </c>
       <c r="N17">
         <v>21485412</v>
       </c>
@@ -2618,7 +2645,10 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>240</v>
+      </c>
       <c r="N18">
         <v>84754121</v>
       </c>
@@ -2638,7 +2668,10 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>210</v>
+      </c>
       <c r="N19">
         <v>26958745</v>
       </c>
@@ -2655,7 +2688,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>241</v>
+      </c>
       <c r="N20">
         <v>24857451</v>
       </c>
@@ -2672,7 +2708,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>211</v>
+      </c>
       <c r="N21">
         <v>26968751</v>
       </c>
@@ -2692,7 +2731,10 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>242</v>
+      </c>
       <c r="N22">
         <v>26745841</v>
       </c>
@@ -2709,7 +2751,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:23" x14ac:dyDescent="0.25">
       <c r="N23">
         <v>28451256</v>
       </c>
@@ -2729,7 +2771,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="24" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:23" x14ac:dyDescent="0.25">
       <c r="N24">
         <v>27451254</v>
       </c>
@@ -2749,7 +2791,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:23" x14ac:dyDescent="0.25">
       <c r="N25">
         <v>23569854</v>
       </c>
@@ -2766,7 +2808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:23" x14ac:dyDescent="0.25">
       <c r="N26">
         <v>24785954</v>
       </c>
@@ -2786,7 +2828,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:23" x14ac:dyDescent="0.25">
       <c r="N27">
         <v>26958354</v>
       </c>
@@ -2803,7 +2845,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="14:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:23" x14ac:dyDescent="0.25">
       <c r="N28">
         <v>21253687</v>
       </c>
@@ -2861,21 +2903,21 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="17" t="s">
         <v>230</v>
       </c>
       <c r="I3" s="14"/>
@@ -2884,16 +2926,16 @@
       </c>
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="Q3" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="R3" s="31" t="s">
+      <c r="R3" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="S3" s="31" t="s">
+      <c r="S3" s="23" t="s">
         <v>230</v>
       </c>
       <c r="T3" s="14"/>
@@ -2902,42 +2944,42 @@
       <c r="B4" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="21">
+      <c r="D4" s="35"/>
+      <c r="E4" s="17">
         <v>7</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="17">
         <v>3</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="17">
         <f>E4*100/(E4+F4)</f>
         <v>70</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="17">
         <f>10-E4-F4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="N4" s="33" t="s">
+      <c r="N4" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="31">
+      <c r="O4" s="31"/>
+      <c r="P4" s="23">
         <v>9</v>
       </c>
-      <c r="Q4" s="31">
+      <c r="Q4" s="23">
         <v>0</v>
       </c>
-      <c r="R4" s="31">
+      <c r="R4" s="23">
         <f>P4*100/(P4+Q4)</f>
         <v>100</v>
       </c>
-      <c r="S4" s="31">
+      <c r="S4" s="23">
         <f>10-P4-Q4</f>
         <v>1</v>
       </c>
@@ -2946,42 +2988,42 @@
       <c r="B5" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="21">
+      <c r="D5" s="35"/>
+      <c r="E5" s="17">
         <v>9</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="17">
         <v>1</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="17">
         <f t="shared" ref="G5:G8" si="0">E5*100/(E5+F5)</f>
         <v>90</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="17">
         <f t="shared" ref="H5:H8" si="1">10-E5-F5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="N5" s="33" t="s">
+      <c r="N5" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="O5" s="33"/>
-      <c r="P5" s="31">
+      <c r="O5" s="31"/>
+      <c r="P5" s="23">
         <v>9</v>
       </c>
-      <c r="Q5" s="31">
+      <c r="Q5" s="23">
         <v>1</v>
       </c>
-      <c r="R5" s="31">
+      <c r="R5" s="23">
         <f t="shared" ref="R5:R8" si="2">P5*100/(P5+Q5)</f>
         <v>90</v>
       </c>
-      <c r="S5" s="31">
+      <c r="S5" s="23">
         <f t="shared" ref="S5:S8" si="3">10-P5-Q5</f>
         <v>0</v>
       </c>
@@ -2990,42 +3032,42 @@
       <c r="B6" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="21">
+      <c r="D6" s="35"/>
+      <c r="E6" s="17">
         <v>6</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="17">
         <v>4</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="17">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="N6" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="O6" s="33"/>
-      <c r="P6" s="31">
+      <c r="O6" s="31"/>
+      <c r="P6" s="23">
         <v>8</v>
       </c>
-      <c r="Q6" s="31">
+      <c r="Q6" s="23">
         <v>2</v>
       </c>
-      <c r="R6" s="31">
+      <c r="R6" s="23">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="S6" s="31">
+      <c r="S6" s="23">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3034,42 +3076,42 @@
       <c r="B7" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="21">
+      <c r="D7" s="35"/>
+      <c r="E7" s="17">
         <v>3</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="17">
         <v>4</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="17">
         <f t="shared" si="0"/>
         <v>42.857142857142854</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="17">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="24" t="s">
         <v>221</v>
       </c>
-      <c r="N7" s="33" t="s">
+      <c r="N7" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="O7" s="33"/>
-      <c r="P7" s="31">
+      <c r="O7" s="31"/>
+      <c r="P7" s="23">
         <v>4</v>
       </c>
-      <c r="Q7" s="31">
+      <c r="Q7" s="23">
         <v>3</v>
       </c>
-      <c r="R7" s="31">
+      <c r="R7" s="23">
         <f t="shared" si="2"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="S7" s="31">
+      <c r="S7" s="23">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
@@ -3078,493 +3120,507 @@
       <c r="B8" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="21">
+      <c r="D8" s="35"/>
+      <c r="E8" s="17">
         <v>7</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="17">
         <v>0</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="17">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="17">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M8" s="32" t="s">
+      <c r="M8" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="N8" s="33" t="s">
+      <c r="N8" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="O8" s="33"/>
-      <c r="P8" s="31">
+      <c r="O8" s="31"/>
+      <c r="P8" s="23">
         <v>8</v>
       </c>
-      <c r="Q8" s="31">
+      <c r="Q8" s="23">
         <v>1</v>
       </c>
-      <c r="R8" s="31">
+      <c r="R8" s="23">
         <f t="shared" si="2"/>
         <v>88.888888888888886</v>
       </c>
-      <c r="S8" s="31">
+      <c r="S8" s="23">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G9" s="22">
+      <c r="G9" s="18">
         <f>SUM(E4:E8)*100/(SUM(E4:E8)+SUM(F4:F8))</f>
         <v>72.727272727272734</v>
       </c>
-      <c r="R9" s="22">
+      <c r="R9" s="18">
         <f>SUM(P4:P8)*100/(SUM(P4:P8)+SUM(Q4:Q8))</f>
         <v>84.444444444444443</v>
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G10" s="23">
+      <c r="G10" s="19">
         <f>100-G9</f>
         <v>27.272727272727266</v>
       </c>
-      <c r="R10" s="23">
+      <c r="R10" s="19">
         <f>100-R9</f>
         <v>15.555555555555557</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="20" t="s">
         <v>230</v>
       </c>
       <c r="I14" s="14"/>
-      <c r="M14" s="34" t="s">
+      <c r="M14" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="35" t="s">
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="Q14" s="35" t="s">
+      <c r="Q14" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="R14" s="35" t="s">
+      <c r="R14" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="S14" s="35" t="s">
+      <c r="S14" s="25" t="s">
         <v>230</v>
       </c>
       <c r="T14" s="14"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="33" t="s">
         <v>218</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="25">
+      <c r="D15" s="33"/>
+      <c r="E15" s="20">
         <v>4</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="20">
         <v>5</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="20">
         <f>E15*100/(E15+F15)</f>
         <v>44.444444444444443</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="20">
         <f>10-E15-F15</f>
         <v>1</v>
       </c>
       <c r="M15" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="N15" s="16" t="s">
+      <c r="N15" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="O15" s="16"/>
-      <c r="P15" s="35">
+      <c r="O15" s="28"/>
+      <c r="P15" s="25">
         <v>10</v>
       </c>
-      <c r="Q15" s="35">
+      <c r="Q15" s="25">
         <v>0</v>
       </c>
-      <c r="R15" s="35">
+      <c r="R15" s="25">
         <f>P15*100/(P15+Q15)</f>
         <v>100</v>
       </c>
-      <c r="S15" s="35">
+      <c r="S15" s="25">
         <f>10-P15-Q15</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="25">
+      <c r="D16" s="33"/>
+      <c r="E16" s="20">
         <v>10</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="20">
         <v>0</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="20">
         <f t="shared" ref="G16:G19" si="4">E16*100/(E16+F16)</f>
         <v>100</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="20">
         <f t="shared" ref="H16:H19" si="5">10-E16-F16</f>
         <v>0</v>
       </c>
       <c r="M16" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="N16" s="16" t="s">
+      <c r="N16" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="O16" s="16"/>
-      <c r="P16" s="35">
+      <c r="O16" s="28"/>
+      <c r="P16" s="25">
         <v>10</v>
       </c>
-      <c r="Q16" s="35">
+      <c r="Q16" s="25">
         <v>0</v>
       </c>
-      <c r="R16" s="35">
+      <c r="R16" s="25">
         <f t="shared" ref="R16:R19" si="6">P16*100/(P16+Q16)</f>
         <v>100</v>
       </c>
-      <c r="S16" s="35">
+      <c r="S16" s="25">
         <f t="shared" ref="S16:S19" si="7">10-P16-Q16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="25">
+      <c r="D17" s="33"/>
+      <c r="E17" s="20">
         <v>7</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="20">
         <v>1</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="20">
         <f t="shared" si="4"/>
         <v>87.5</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="20">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="M17" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="N17" s="16" t="s">
+      <c r="N17" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="O17" s="16"/>
-      <c r="P17" s="35">
+      <c r="O17" s="28"/>
+      <c r="P17" s="25">
         <v>9</v>
       </c>
-      <c r="Q17" s="35">
+      <c r="Q17" s="25">
         <v>1</v>
       </c>
-      <c r="R17" s="35">
+      <c r="R17" s="25">
         <f t="shared" si="6"/>
         <v>90</v>
       </c>
-      <c r="S17" s="35">
+      <c r="S17" s="25">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="25">
+      <c r="D18" s="33"/>
+      <c r="E18" s="20">
         <v>1</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="20">
         <v>6</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="20">
         <f t="shared" si="4"/>
         <v>14.285714285714286</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="20">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="M18" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="N18" s="16" t="s">
+      <c r="N18" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="O18" s="16"/>
-      <c r="P18" s="35">
+      <c r="O18" s="28"/>
+      <c r="P18" s="25">
         <v>7</v>
       </c>
-      <c r="Q18" s="35">
+      <c r="Q18" s="25">
         <v>0</v>
       </c>
-      <c r="R18" s="35">
+      <c r="R18" s="25">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="S18" s="35">
+      <c r="S18" s="25">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="25">
+      <c r="D19" s="33"/>
+      <c r="E19" s="20">
         <v>4</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="20">
         <v>4</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="20">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="20">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="M19" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="N19" s="16" t="s">
+      <c r="N19" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="O19" s="16"/>
-      <c r="P19" s="35">
+      <c r="O19" s="28"/>
+      <c r="P19" s="25">
         <v>6</v>
       </c>
-      <c r="Q19" s="35">
+      <c r="Q19" s="25">
         <v>3</v>
       </c>
-      <c r="R19" s="35">
+      <c r="R19" s="25">
         <f t="shared" si="6"/>
         <v>66.666666666666671</v>
       </c>
-      <c r="S19" s="35">
+      <c r="S19" s="25">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G20" s="22">
+      <c r="G20" s="18">
         <f>SUM(E15:E19)*100/(SUM(E15:E19)+SUM(F15:F19))</f>
         <v>61.904761904761905</v>
       </c>
-      <c r="R20" s="22">
+      <c r="R20" s="18">
         <f>SUM(P15:P19)*100/(SUM(P15:P19)+SUM(Q15:Q19))</f>
         <v>91.304347826086953</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G21" s="23">
+      <c r="G21" s="19">
         <f>100-G20</f>
         <v>38.095238095238095</v>
       </c>
-      <c r="R21" s="23">
+      <c r="R21" s="19">
         <f>100-R20</f>
         <v>8.6956521739130466</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27" t="s">
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H25" s="21" t="s">
         <v>230</v>
       </c>
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="22" t="s">
         <v>217</v>
       </c>
       <c r="C26" s="29" t="s">
         <v>218</v>
       </c>
       <c r="D26" s="29"/>
-      <c r="E26" s="27">
+      <c r="E26" s="21">
         <v>9</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="21">
         <v>1</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="21">
         <f>E26*100/(E26+F26)</f>
         <v>90</v>
       </c>
-      <c r="H26" s="27">
+      <c r="H26" s="21">
         <f>10-E26-F26</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="22" t="s">
         <v>219</v>
       </c>
       <c r="C27" s="29" t="s">
         <v>223</v>
       </c>
       <c r="D27" s="29"/>
-      <c r="E27" s="27">
+      <c r="E27" s="21">
         <v>5</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="21">
         <v>3</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="21">
         <f t="shared" ref="G27:G30" si="8">E27*100/(E27+F27)</f>
         <v>62.5</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27" s="21">
         <f t="shared" ref="H27:H30" si="9">10-E27-F27</f>
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="22" t="s">
         <v>220</v>
       </c>
       <c r="C28" s="29" t="s">
         <v>224</v>
       </c>
       <c r="D28" s="29"/>
-      <c r="E28" s="27">
+      <c r="E28" s="21">
         <v>7</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="21">
         <v>0</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="21">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="21">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="22" t="s">
         <v>221</v>
       </c>
       <c r="C29" s="29" t="s">
         <v>225</v>
       </c>
       <c r="D29" s="29"/>
-      <c r="E29" s="27">
+      <c r="E29" s="21">
         <v>10</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="21">
         <v>0</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="21">
         <f t="shared" si="8"/>
         <v>100</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="21">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="22" t="s">
         <v>222</v>
       </c>
       <c r="C30" s="29" t="s">
         <v>226</v>
       </c>
       <c r="D30" s="29"/>
-      <c r="E30" s="27">
+      <c r="E30" s="21">
         <v>6</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F30" s="21">
         <v>3</v>
       </c>
-      <c r="G30" s="27">
+      <c r="G30" s="21">
         <f t="shared" si="8"/>
         <v>66.666666666666671</v>
       </c>
-      <c r="H30" s="27">
+      <c r="H30" s="21">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G31" s="22">
+      <c r="G31" s="18">
         <f>SUM(E26:E30)*100/(SUM(E26:E30)+SUM(F26:F30))</f>
         <v>84.090909090909093</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G32" s="23">
+      <c r="G32" s="19">
         <f>100-G31</f>
         <v>15.909090909090907</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="N19:O19"/>
@@ -3581,20 +3637,6 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3621,21 +3663,21 @@
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21" t="s">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="17" t="s">
         <v>230</v>
       </c>
       <c r="I3" s="14"/>
@@ -3644,16 +3686,16 @@
       </c>
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="Q3" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="R3" s="31" t="s">
+      <c r="R3" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="S3" s="31" t="s">
+      <c r="S3" s="23" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3661,43 +3703,43 @@
       <c r="B4" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="21">
+      <c r="D4" s="35"/>
+      <c r="E4" s="17">
         <v>9</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="17">
         <v>1</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="17">
         <f>E4*100/(E4+F4)</f>
         <v>90</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="17">
         <f>10-E4-F4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="32" t="str">
+      <c r="M4" s="24" t="str">
         <f t="shared" ref="M4:M8" si="0">B4</f>
         <v>C1</v>
       </c>
-      <c r="N4" s="33" t="s">
+      <c r="N4" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="O4" s="33"/>
-      <c r="P4" s="31">
+      <c r="O4" s="31"/>
+      <c r="P4" s="23">
         <v>4</v>
       </c>
-      <c r="Q4" s="31">
+      <c r="Q4" s="23">
         <v>2</v>
       </c>
-      <c r="R4" s="31">
+      <c r="R4" s="23">
         <f>P4*100/(P4+Q4)</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="S4" s="31">
+      <c r="S4" s="23">
         <f>10-P4-Q4</f>
         <v>4</v>
       </c>
@@ -3706,43 +3748,43 @@
       <c r="B5" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="21">
+      <c r="D5" s="35"/>
+      <c r="E5" s="17">
         <v>8</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="17">
         <v>2</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="17">
         <f t="shared" ref="G5:G8" si="1">E5*100/(E5+F5)</f>
         <v>80</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="17">
         <f t="shared" ref="H5:H8" si="2">10-E5-F5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="32" t="str">
+      <c r="M5" s="24" t="str">
         <f t="shared" si="0"/>
         <v>C2</v>
       </c>
-      <c r="N5" s="33" t="s">
+      <c r="N5" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="O5" s="33"/>
-      <c r="P5" s="31">
+      <c r="O5" s="31"/>
+      <c r="P5" s="23">
         <v>7</v>
       </c>
-      <c r="Q5" s="31">
+      <c r="Q5" s="23">
         <v>2</v>
       </c>
-      <c r="R5" s="31">
+      <c r="R5" s="23">
         <f t="shared" ref="R5:R8" si="3">P5*100/(P5+Q5)</f>
         <v>77.777777777777771</v>
       </c>
-      <c r="S5" s="31">
+      <c r="S5" s="23">
         <f t="shared" ref="S5:S8" si="4">10-P5-Q5</f>
         <v>1</v>
       </c>
@@ -3751,43 +3793,43 @@
       <c r="B6" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="21">
+      <c r="D6" s="35"/>
+      <c r="E6" s="17">
         <v>1</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="17">
         <v>9</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="17">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M6" s="32" t="str">
+      <c r="M6" s="24" t="str">
         <f t="shared" si="0"/>
         <v>C3</v>
       </c>
-      <c r="N6" s="33" t="s">
+      <c r="N6" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="O6" s="33"/>
-      <c r="P6" s="31">
+      <c r="O6" s="31"/>
+      <c r="P6" s="23">
         <v>10</v>
       </c>
-      <c r="Q6" s="31">
+      <c r="Q6" s="23">
         <v>0</v>
       </c>
-      <c r="R6" s="31">
+      <c r="R6" s="23">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="S6" s="31">
+      <c r="S6" s="23">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -3796,43 +3838,43 @@
       <c r="B7" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="21">
+      <c r="D7" s="35"/>
+      <c r="E7" s="17">
         <v>5</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="17">
         <v>5</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="17">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M7" s="32" t="str">
+      <c r="M7" s="24" t="str">
         <f t="shared" si="0"/>
         <v>C4</v>
       </c>
-      <c r="N7" s="33" t="s">
+      <c r="N7" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="O7" s="33"/>
-      <c r="P7" s="31">
+      <c r="O7" s="31"/>
+      <c r="P7" s="23">
         <v>5</v>
       </c>
-      <c r="Q7" s="31">
+      <c r="Q7" s="23">
         <v>4</v>
       </c>
-      <c r="R7" s="31">
+      <c r="R7" s="23">
         <f t="shared" si="3"/>
         <v>55.555555555555557</v>
       </c>
-      <c r="S7" s="31">
+      <c r="S7" s="23">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -3841,112 +3883,112 @@
       <c r="B8" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="21">
+      <c r="D8" s="35"/>
+      <c r="E8" s="17">
         <v>4</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="17">
         <v>3</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="17">
         <f t="shared" si="1"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="17">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="M8" s="32" t="str">
+      <c r="M8" s="24" t="str">
         <f t="shared" si="0"/>
         <v>C5</v>
       </c>
-      <c r="N8" s="33" t="s">
+      <c r="N8" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="O8" s="33"/>
-      <c r="P8" s="31">
+      <c r="O8" s="31"/>
+      <c r="P8" s="23">
         <v>5</v>
       </c>
-      <c r="Q8" s="31">
+      <c r="Q8" s="23">
         <v>5</v>
       </c>
-      <c r="R8" s="31">
+      <c r="R8" s="23">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="S8" s="31">
+      <c r="S8" s="23">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G9" s="36"/>
-      <c r="R9" s="36"/>
+      <c r="G9" s="26"/>
+      <c r="R9" s="26"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G10" s="36"/>
-      <c r="R10" s="36"/>
+      <c r="G10" s="26"/>
+      <c r="R10" s="26"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="25" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="20" t="s">
         <v>228</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="20" t="s">
         <v>230</v>
       </c>
       <c r="I14" s="14"/>
-      <c r="M14" s="34" t="s">
+      <c r="M14" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="35" t="s">
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="Q14" s="35" t="s">
+      <c r="Q14" s="25" t="s">
         <v>228</v>
       </c>
-      <c r="R14" s="35" t="s">
+      <c r="R14" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="S14" s="35" t="s">
+      <c r="S14" s="25" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="str">
+      <c r="B15" s="16" t="str">
         <f t="shared" ref="B15:B19" si="5">B4</f>
         <v>C1</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="33" t="s">
         <v>218</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="25">
+      <c r="D15" s="33"/>
+      <c r="E15" s="20">
         <v>8</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="20">
         <v>1</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="20">
         <f>E15*100/(E15+F15)</f>
         <v>88.888888888888886</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H15" s="20">
         <f>10-E15-F15</f>
         <v>1</v>
       </c>
@@ -3954,45 +3996,45 @@
         <f t="shared" ref="M15:M19" si="6">B4</f>
         <v>C1</v>
       </c>
-      <c r="N15" s="16" t="s">
+      <c r="N15" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="O15" s="16"/>
-      <c r="P15" s="35">
+      <c r="O15" s="28"/>
+      <c r="P15" s="25">
         <v>4</v>
       </c>
-      <c r="Q15" s="35">
+      <c r="Q15" s="25">
         <v>3</v>
       </c>
-      <c r="R15" s="35">
+      <c r="R15" s="25">
         <f>P15*100/(P15+Q15)</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="S15" s="35">
+      <c r="S15" s="25">
         <f>10-P15-Q15</f>
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="str">
+      <c r="B16" s="16" t="str">
         <f t="shared" si="5"/>
         <v>C2</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="25">
+      <c r="D16" s="33"/>
+      <c r="E16" s="20">
         <v>7</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="20">
         <v>3</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="20">
         <f t="shared" ref="G16:G19" si="7">E16*100/(E16+F16)</f>
         <v>70</v>
       </c>
-      <c r="H16" s="25">
+      <c r="H16" s="20">
         <f t="shared" ref="H16:H19" si="8">10-E16-F16</f>
         <v>0</v>
       </c>
@@ -4000,45 +4042,45 @@
         <f t="shared" si="6"/>
         <v>C2</v>
       </c>
-      <c r="N16" s="16" t="s">
+      <c r="N16" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="O16" s="16"/>
-      <c r="P16" s="35">
+      <c r="O16" s="28"/>
+      <c r="P16" s="25">
         <v>9</v>
       </c>
-      <c r="Q16" s="35">
+      <c r="Q16" s="25">
         <v>1</v>
       </c>
-      <c r="R16" s="35">
+      <c r="R16" s="25">
         <f t="shared" ref="R16:R19" si="9">P16*100/(P16+Q16)</f>
         <v>90</v>
       </c>
-      <c r="S16" s="35">
+      <c r="S16" s="25">
         <f t="shared" ref="S16:S19" si="10">10-P16-Q16</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="str">
+      <c r="B17" s="16" t="str">
         <f t="shared" si="5"/>
         <v>C3</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="33" t="s">
         <v>224</v>
       </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="25">
+      <c r="D17" s="33"/>
+      <c r="E17" s="20">
         <v>9</v>
       </c>
-      <c r="F17" s="25">
+      <c r="F17" s="20">
         <v>0</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="20">
         <f t="shared" si="7"/>
         <v>100</v>
       </c>
-      <c r="H17" s="25">
+      <c r="H17" s="20">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
@@ -4046,45 +4088,45 @@
         <f t="shared" si="6"/>
         <v>C3</v>
       </c>
-      <c r="N17" s="16" t="s">
+      <c r="N17" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="O17" s="16"/>
-      <c r="P17" s="35">
+      <c r="O17" s="28"/>
+      <c r="P17" s="25">
         <v>7</v>
       </c>
-      <c r="Q17" s="35">
+      <c r="Q17" s="25">
         <v>2</v>
       </c>
-      <c r="R17" s="35">
+      <c r="R17" s="25">
         <f t="shared" si="9"/>
         <v>77.777777777777771</v>
       </c>
-      <c r="S17" s="35">
+      <c r="S17" s="25">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="str">
+      <c r="B18" s="16" t="str">
         <f t="shared" si="5"/>
         <v>C4</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="33" t="s">
         <v>225</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="E18" s="25">
+      <c r="D18" s="33"/>
+      <c r="E18" s="20">
         <v>5</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="20">
         <v>3</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="20">
         <f t="shared" si="7"/>
         <v>62.5</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="20">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
@@ -4092,45 +4134,45 @@
         <f t="shared" si="6"/>
         <v>C4</v>
       </c>
-      <c r="N18" s="16" t="s">
+      <c r="N18" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="O18" s="16"/>
-      <c r="P18" s="35">
+      <c r="O18" s="28"/>
+      <c r="P18" s="25">
         <v>9</v>
       </c>
-      <c r="Q18" s="35">
+      <c r="Q18" s="25">
         <v>0</v>
       </c>
-      <c r="R18" s="35">
+      <c r="R18" s="25">
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="S18" s="35">
+      <c r="S18" s="25">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="str">
+      <c r="B19" s="16" t="str">
         <f t="shared" si="5"/>
         <v>C5</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="D19" s="19"/>
-      <c r="E19" s="25">
+      <c r="D19" s="33"/>
+      <c r="E19" s="20">
         <v>7</v>
       </c>
-      <c r="F19" s="25">
+      <c r="F19" s="20">
         <v>2</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="20">
         <f t="shared" si="7"/>
         <v>77.777777777777771</v>
       </c>
-      <c r="H19" s="25">
+      <c r="H19" s="20">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
@@ -4138,59 +4180,59 @@
         <f t="shared" si="6"/>
         <v>C5</v>
       </c>
-      <c r="N19" s="16" t="s">
+      <c r="N19" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="O19" s="16"/>
-      <c r="P19" s="35">
+      <c r="O19" s="28"/>
+      <c r="P19" s="25">
         <v>10</v>
       </c>
-      <c r="Q19" s="35">
+      <c r="Q19" s="25">
         <v>0</v>
       </c>
-      <c r="R19" s="35">
+      <c r="R19" s="25">
         <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="S19" s="35">
+      <c r="S19" s="25">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G20" s="36"/>
-      <c r="R20" s="36"/>
+      <c r="G20" s="26"/>
+      <c r="R20" s="26"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G21" s="36"/>
-      <c r="R21" s="36"/>
+      <c r="G21" s="26"/>
+      <c r="R21" s="26"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G22" s="37"/>
-      <c r="R22" s="37"/>
+      <c r="G22" s="27"/>
+      <c r="R22" s="27"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="27" t="s">
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="H25" s="27" t="s">
+      <c r="H25" s="21" t="s">
         <v>230</v>
       </c>
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="str">
+      <c r="B26" s="22" t="str">
         <f t="shared" ref="B26:B30" si="11">B4</f>
         <v>C1</v>
       </c>
@@ -4198,23 +4240,23 @@
         <v>218</v>
       </c>
       <c r="D26" s="29"/>
-      <c r="E26" s="27">
+      <c r="E26" s="21">
         <v>4</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="21">
         <v>5</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="21">
         <f>E26*100/(E26+F26)</f>
         <v>44.444444444444443</v>
       </c>
-      <c r="H26" s="27">
+      <c r="H26" s="21">
         <f>10-E26-F26</f>
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="str">
+      <c r="B27" s="22" t="str">
         <f t="shared" si="11"/>
         <v>C2</v>
       </c>
@@ -4222,23 +4264,23 @@
         <v>223</v>
       </c>
       <c r="D27" s="29"/>
-      <c r="E27" s="27">
+      <c r="E27" s="21">
         <v>8</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="21">
         <v>1</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="21">
         <f t="shared" ref="G27:G30" si="12">E27*100/(E27+F27)</f>
         <v>88.888888888888886</v>
       </c>
-      <c r="H27" s="27">
+      <c r="H27" s="21">
         <f t="shared" ref="H27:H30" si="13">10-E27-F27</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="28" t="str">
+      <c r="B28" s="22" t="str">
         <f t="shared" si="11"/>
         <v>C3</v>
       </c>
@@ -4246,23 +4288,23 @@
         <v>224</v>
       </c>
       <c r="D28" s="29"/>
-      <c r="E28" s="27">
+      <c r="E28" s="21">
         <v>9</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="21">
         <v>0</v>
       </c>
-      <c r="G28" s="27">
+      <c r="G28" s="21">
         <f t="shared" si="12"/>
         <v>100</v>
       </c>
-      <c r="H28" s="27">
+      <c r="H28" s="21">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="str">
+      <c r="B29" s="22" t="str">
         <f t="shared" si="11"/>
         <v>C4</v>
       </c>
@@ -4270,23 +4312,23 @@
         <v>225</v>
       </c>
       <c r="D29" s="29"/>
-      <c r="E29" s="27">
+      <c r="E29" s="21">
         <v>10</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="21">
         <v>0</v>
       </c>
-      <c r="G29" s="27">
+      <c r="G29" s="21">
         <f t="shared" si="12"/>
         <v>100</v>
       </c>
-      <c r="H29" s="27">
+      <c r="H29" s="21">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="str">
+      <c r="B30" s="22" t="str">
         <f t="shared" si="11"/>
         <v>C5</v>
       </c>
@@ -4294,37 +4336,50 @@
         <v>226</v>
       </c>
       <c r="D30" s="29"/>
-      <c r="E30" s="27">
+      <c r="E30" s="21">
         <v>3</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F30" s="21">
         <v>6</v>
       </c>
-      <c r="G30" s="27">
+      <c r="G30" s="21">
         <f t="shared" si="12"/>
         <v>33.333333333333336</v>
       </c>
-      <c r="H30" s="27">
+      <c r="H30" s="21">
         <f t="shared" si="13"/>
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G31" s="36"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G32" s="36"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="37"/>
+      <c r="G33" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="N16:O16"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="N17:O17"/>
@@ -4332,24 +4387,11 @@
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="N19:O19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>